<commit_message>
Update Visualization Courses Schedule.xlsx
</commit_message>
<xml_diff>
--- a/Week1/Visualization Courses Schedule.xlsx
+++ b/Week1/Visualization Courses Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timsmac/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timsmac/Documents/GitHub/HRL-at-NYUSH/data-viz-mining/Week1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F8C2EC-DF30-6846-BE36-BE3FB7170FC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8556B51-D620-EF4A-81BA-93E71DE03897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="460" windowWidth="25060" windowHeight="13360" activeTab="2" xr2:uid="{6E486159-7906-AA4D-91AE-D6A687DA1629}"/>
+    <workbookView xWindow="540" yWindow="460" windowWidth="25060" windowHeight="13360" xr2:uid="{6E486159-7906-AA4D-91AE-D6A687DA1629}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Timeline - Theme" sheetId="1" r:id="rId1"/>
@@ -1076,7 +1076,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3DF842E-27A6-754F-8D08-E64C4D5B8477}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView zoomScale="61" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="61" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1155,7 +1157,7 @@
       <c r="G2" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="13" t="s">
         <v>72</v>
       </c>
       <c r="I2" s="17" t="s">
@@ -1190,7 +1192,7 @@
       <c r="G3" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="13" t="s">
         <v>73</v>
       </c>
       <c r="I3" s="6" t="s">
@@ -2716,7 +2718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AEAF844-66D6-3F48-9C30-5C7929ADA466}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Revert "Draft W4 note"
This reverts commit 373213b1ea6d67b3464b9a1cf613d9a39874d5aa.
</commit_message>
<xml_diff>
--- a/Week1/Visualization Courses Schedule.xlsx
+++ b/Week1/Visualization Courses Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timsmac/Documents/GitHub/HRL-at-NYUSH/data-viz-mining/Week1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E68C88D-B132-A34C-A66C-2FB23961697A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8556B51-D620-EF4A-81BA-93E71DE03897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="600" windowWidth="16840" windowHeight="13100" xr2:uid="{6E486159-7906-AA4D-91AE-D6A687DA1629}"/>
+    <workbookView xWindow="540" yWindow="460" windowWidth="25060" windowHeight="13360" xr2:uid="{6E486159-7906-AA4D-91AE-D6A687DA1629}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Timeline - Theme" sheetId="1" r:id="rId1"/>
@@ -1076,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3DF842E-27A6-754F-8D08-E64C4D5B8477}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="61" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Revert "Revert "Draft W4 note""
This reverts commit 8be542137b2cea5c4635a82540b549b271b5f7f7.
</commit_message>
<xml_diff>
--- a/Week1/Visualization Courses Schedule.xlsx
+++ b/Week1/Visualization Courses Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timsmac/Documents/GitHub/HRL-at-NYUSH/data-viz-mining/Week1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8556B51-D620-EF4A-81BA-93E71DE03897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E68C88D-B132-A34C-A66C-2FB23961697A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="460" windowWidth="25060" windowHeight="13360" xr2:uid="{6E486159-7906-AA4D-91AE-D6A687DA1629}"/>
+    <workbookView xWindow="8220" yWindow="600" windowWidth="16840" windowHeight="13100" xr2:uid="{6E486159-7906-AA4D-91AE-D6A687DA1629}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Timeline - Theme" sheetId="1" r:id="rId1"/>
@@ -1076,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3DF842E-27A6-754F-8D08-E64C4D5B8477}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="61" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adjust course column order
</commit_message>
<xml_diff>
--- a/Week1/Visualization Courses Schedule.xlsx
+++ b/Week1/Visualization Courses Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timsmac/Documents/GitHub/HRL-at-NYUSH/data-viz-mining/Week1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E68C88D-B132-A34C-A66C-2FB23961697A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9464D480-286E-164A-88C8-83F0FC436817}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8220" yWindow="600" windowWidth="16840" windowHeight="13100" xr2:uid="{6E486159-7906-AA4D-91AE-D6A687DA1629}"/>
   </bookViews>
@@ -1076,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3DF842E-27A6-754F-8D08-E64C4D5B8477}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1090,8 +1090,8 @@
     <col min="9" max="9" width="39.1640625" customWidth="1"/>
     <col min="10" max="10" width="47.5" customWidth="1"/>
     <col min="11" max="11" width="36.1640625" customWidth="1"/>
-    <col min="12" max="12" width="32" customWidth="1"/>
-    <col min="13" max="13" width="62.5" customWidth="1"/>
+    <col min="12" max="12" width="62.5" customWidth="1"/>
+    <col min="13" max="13" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1129,10 +1129,10 @@
         <v>141</v>
       </c>
       <c r="L1" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="M1" s="19" t="s">
         <v>142</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1201,7 +1201,7 @@
       <c r="J3" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="M3" t="s">
+      <c r="L3" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1236,11 +1236,11 @@
       <c r="K4" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="M4" s="17" t="s">
         <v>135</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1268,7 +1268,7 @@
       <c r="J5" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="M5" t="s">
+      <c r="L5" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1303,11 +1303,11 @@
       <c r="K6" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1335,7 +1335,7 @@
       <c r="J7" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="M7" t="s">
+      <c r="L7" t="s">
         <v>157</v>
       </c>
     </row>
@@ -1370,11 +1370,11 @@
       <c r="K8" t="s">
         <v>128</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="M8" s="15" t="s">
         <v>137</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1402,7 +1402,7 @@
       <c r="J9" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="M9" t="s">
+      <c r="L9" t="s">
         <v>156</v>
       </c>
     </row>
@@ -1440,11 +1440,11 @@
       <c r="K10" t="s">
         <v>129</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="M10" s="13" t="s">
         <v>138</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1472,7 +1472,7 @@
       <c r="J11" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="M11" t="s">
+      <c r="L11" t="s">
         <v>155</v>
       </c>
     </row>
@@ -1507,11 +1507,11 @@
       <c r="K12" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="L12" s="14" t="s">
+      <c r="L12" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="14" t="s">
         <v>139</v>
-      </c>
-      <c r="M12" s="18" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1539,7 +1539,7 @@
       <c r="J13" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="M13" t="s">
+      <c r="L13" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1572,10 +1572,10 @@
         <v>131</v>
       </c>
       <c r="L14" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" t="s">
         <v>140</v>
-      </c>
-      <c r="M14" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1600,7 +1600,7 @@
       <c r="J15" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="M15" t="s">
+      <c r="L15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1632,11 +1632,11 @@
       <c r="K16" t="s">
         <v>132</v>
       </c>
-      <c r="M16" t="s">
+      <c r="L16" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17">
         <v>16</v>
       </c>
@@ -1658,11 +1658,11 @@
       <c r="J17" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="M17" t="s">
+      <c r="L17" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1693,11 +1693,11 @@
       <c r="K18" t="s">
         <v>133</v>
       </c>
-      <c r="M18" s="16" t="s">
+      <c r="L18" s="16" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19">
         <v>18</v>
       </c>
@@ -1719,11 +1719,11 @@
       <c r="J19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M19" t="s">
+      <c r="L19" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>10</v>
       </c>
@@ -1748,11 +1748,11 @@
       <c r="K20" t="s">
         <v>134</v>
       </c>
-      <c r="M20" s="12" t="s">
+      <c r="L20" s="12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21">
         <v>20</v>
       </c>
@@ -1771,11 +1771,11 @@
       <c r="J21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="M21" t="s">
+      <c r="L21" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>11</v>
       </c>
@@ -1794,11 +1794,11 @@
       <c r="J22" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="M22" t="s">
+      <c r="L22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23">
         <v>22</v>
       </c>
@@ -1814,11 +1814,11 @@
       <c r="J23" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="M23" t="s">
+      <c r="L23" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>12</v>
       </c>
@@ -1837,11 +1837,11 @@
       <c r="J24" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="M24" t="s">
+      <c r="L24" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25">
         <v>24</v>
       </c>
@@ -1857,11 +1857,11 @@
       <c r="J25" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="M25" t="s">
+      <c r="L25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C27">
         <v>26</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>14</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C29">
         <v>28</v>
       </c>
@@ -1911,8 +1911,8 @@
     <hyperlink ref="I1" r:id="rId5" xr:uid="{758B7A86-0744-394F-9909-1FF8264DDC11}"/>
     <hyperlink ref="J1" r:id="rId6" xr:uid="{B3DDADD7-43B7-1345-B0BD-061406BF0C7E}"/>
     <hyperlink ref="K1" r:id="rId7" xr:uid="{FEEBE506-D341-1146-A31D-BF71790B5344}"/>
-    <hyperlink ref="L1" r:id="rId8" xr:uid="{14764646-6D30-184A-A95F-9EF3C1EB2BFD}"/>
-    <hyperlink ref="M1" r:id="rId9" xr:uid="{FC2BD6C4-0ED4-7840-B153-0BAC0D1B83E3}"/>
+    <hyperlink ref="M1" r:id="rId8" xr:uid="{14764646-6D30-184A-A95F-9EF3C1EB2BFD}"/>
+    <hyperlink ref="L1" r:id="rId9" xr:uid="{FC2BD6C4-0ED4-7840-B153-0BAC0D1B83E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>